<commit_message>
with web for test
</commit_message>
<xml_diff>
--- a/voir-spring-boot-angular-server/CATALOG-products.xlsx
+++ b/voir-spring-boot-angular-server/CATALOG-products.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="653">
   <si>
     <t xml:space="preserve">code</t>
   </si>
@@ -1993,6 +1993,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2087,8 +2088,8 @@
   </sheetPr>
   <dimension ref="A1:Q176"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2:M176"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I106" activeCellId="0" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2104,7 +2105,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="117.03"/>
@@ -5226,8 +5227,8 @@
       <c r="H107" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="I107" s="0" t="s">
-        <v>381</v>
+      <c r="I107" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="J107" s="0" t="s">
         <v>315</v>

</xml_diff>